<commit_message>
Updated the database with 10% validation data.
</commit_message>
<xml_diff>
--- a/data/NorthChile/sac/Val.xlsx
+++ b/data/NorthChile/sac/Val.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catal\OneDrive\Escritorio\Repo DNN-HMM\DH-DM-Earthquake-detection\data\NorthChile\sac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catal\OneDrive\Escritorio\DNN-HMM\DH-DM-Earthquake-detection\data\NorthChile\sac\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9E97DA-0292-42D4-87EC-794159A99DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EA793A-8FD7-4695-A782-084EB7BDB7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="406">
   <si>
     <t>name</t>
   </si>
@@ -346,6 +346,75 @@
     <t>H2020_168_VA03_TE</t>
   </si>
   <si>
+    <t>NuevaBase_459_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_460_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_462_PB09</t>
+  </si>
+  <si>
+    <t>NuevaBase_463_PB09</t>
+  </si>
+  <si>
+    <t>NuevaBase_464_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_465_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_467_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_469_PB09</t>
+  </si>
+  <si>
+    <t>NuevaBase_471_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_472_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_473_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_475_PB09</t>
+  </si>
+  <si>
+    <t>NuevaBase_476_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_478_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_479_PB09</t>
+  </si>
+  <si>
+    <t>NuevaBase_480_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_481_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_493_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_494_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_496_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_497_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_498_PB09_TE</t>
+  </si>
+  <si>
+    <t>NuevaBase_501_PB09</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
@@ -451,6 +520,9 @@
     <t>PX06</t>
   </si>
   <si>
+    <t>PB09</t>
+  </si>
+  <si>
     <t>BHE</t>
   </si>
   <si>
@@ -754,6 +826,75 @@
     <t>2020-09-03T04:45:39.000001Z</t>
   </si>
   <si>
+    <t>2019-03-28T15:04:21.000000Z</t>
+  </si>
+  <si>
+    <t>2019-03-28T20:59:01.000001Z</t>
+  </si>
+  <si>
+    <t>2019-04-26T06:20:34.000000Z</t>
+  </si>
+  <si>
+    <t>2019-06-03T08:40:40.000000Z</t>
+  </si>
+  <si>
+    <t>2019-06-14T00:17:32.000000Z</t>
+  </si>
+  <si>
+    <t>2019-08-02T00:07:35.000000Z</t>
+  </si>
+  <si>
+    <t>2019-09-26T20:31:08.000000Z</t>
+  </si>
+  <si>
+    <t>2019-11-04T21:52:45.000000Z</t>
+  </si>
+  <si>
+    <t>2019-12-03T07:27:30.000000Z</t>
+  </si>
+  <si>
+    <t>2019-12-03T08:45:46.000000Z</t>
+  </si>
+  <si>
+    <t>2020-01-09T16:24:40.000000Z</t>
+  </si>
+  <si>
+    <t>2020-02-11T13:49:12.000000Z</t>
+  </si>
+  <si>
+    <t>2020-02-13T05:49:38.000000Z</t>
+  </si>
+  <si>
+    <t>2020-03-30T14:52:34.000000Z</t>
+  </si>
+  <si>
+    <t>2020-04-03T08:46:00.000000Z</t>
+  </si>
+  <si>
+    <t>2020-06-15T04:33:44.000000Z</t>
+  </si>
+  <si>
+    <t>2020-06-19T05:38:36.000000Z</t>
+  </si>
+  <si>
+    <t>2020-10-06T05:15:39.000000Z</t>
+  </si>
+  <si>
+    <t>2020-10-06T11:31:18.000000Z</t>
+  </si>
+  <si>
+    <t>2020-10-21T09:11:36.000001Z</t>
+  </si>
+  <si>
+    <t>2020-10-25T21:15:54.000000Z</t>
+  </si>
+  <si>
+    <t>2020-10-28T14:51:40.000001Z</t>
+  </si>
+  <si>
+    <t>2020-11-21T02:10:10.000000Z</t>
+  </si>
+  <si>
     <t>2020-08-27T03:30:03.000000Z</t>
   </si>
   <si>
@@ -1028,6 +1169,75 @@
   </si>
   <si>
     <t>2020-09-03T05:10:39.000001Z</t>
+  </si>
+  <si>
+    <t>2019-03-28T15:44:15.000000Z</t>
+  </si>
+  <si>
+    <t>2019-03-28T21:08:01.000001Z</t>
+  </si>
+  <si>
+    <t>2019-04-26T06:28:34.000000Z</t>
+  </si>
+  <si>
+    <t>2019-06-03T08:45:52.000000Z</t>
+  </si>
+  <si>
+    <t>2019-06-14T00:48:32.000000Z</t>
+  </si>
+  <si>
+    <t>2019-08-02T00:38:35.000000Z</t>
+  </si>
+  <si>
+    <t>2019-09-26T20:51:08.000000Z</t>
+  </si>
+  <si>
+    <t>2019-11-04T22:02:45.000000Z</t>
+  </si>
+  <si>
+    <t>2019-12-03T07:44:00.000000Z</t>
+  </si>
+  <si>
+    <t>2019-12-03T09:27:46.000000Z</t>
+  </si>
+  <si>
+    <t>2020-01-09T16:44:40.000000Z</t>
+  </si>
+  <si>
+    <t>2020-02-11T13:58:30.000000Z</t>
+  </si>
+  <si>
+    <t>2020-02-13T06:23:44.000000Z</t>
+  </si>
+  <si>
+    <t>2020-03-30T15:06:16.000000Z</t>
+  </si>
+  <si>
+    <t>2020-04-03T08:55:54.000000Z</t>
+  </si>
+  <si>
+    <t>2020-06-15T04:53:44.000000Z</t>
+  </si>
+  <si>
+    <t>2020-06-19T06:02:24.000000Z</t>
+  </si>
+  <si>
+    <t>2020-10-06T05:29:39.000000Z</t>
+  </si>
+  <si>
+    <t>2020-10-06T11:50:18.000000Z</t>
+  </si>
+  <si>
+    <t>2020-10-21T09:18:06.000001Z</t>
+  </si>
+  <si>
+    <t>2020-10-25T21:42:30.000000Z</t>
+  </si>
+  <si>
+    <t>2020-10-28T15:14:40.000001Z</t>
+  </si>
+  <si>
+    <t>2020-11-21T02:19:46.000000Z</t>
   </si>
 </sst>
 </file>
@@ -1109,9 +1319,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1149,9 +1359,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1184,26 +1394,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1236,26 +1429,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1429,13 +1605,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -1462,19 +1641,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="F2" t="s">
-        <v>244</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1482,19 +1661,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s">
-        <v>245</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1502,19 +1681,19 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="F4" t="s">
-        <v>246</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1522,19 +1701,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E5" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="F5" t="s">
-        <v>247</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1542,19 +1721,19 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E6" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
-        <v>248</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1562,19 +1741,19 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="F7" t="s">
-        <v>249</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1582,19 +1761,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E8" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="F8" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -1602,19 +1781,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="F9" t="s">
-        <v>251</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1622,19 +1801,19 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="F10" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -1642,19 +1821,19 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="F11" t="s">
-        <v>252</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -1662,19 +1841,19 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="D12" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="F12" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -1682,19 +1861,19 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E13" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="F13" t="s">
-        <v>253</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -1702,19 +1881,19 @@
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="D14" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E14" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="F14" t="s">
-        <v>254</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1722,19 +1901,19 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E15" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="F15" t="s">
-        <v>255</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1742,19 +1921,19 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="D16" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="F16" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1762,19 +1941,19 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="D17" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E17" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="F17" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1782,19 +1961,19 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E18" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="F18" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1802,19 +1981,19 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="F19" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1822,19 +2001,19 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C20" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E20" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="F20" t="s">
-        <v>256</v>
+        <v>303</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1842,19 +2021,19 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E21" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="F21" t="s">
-        <v>257</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1862,19 +2041,19 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="D22" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E22" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="F22" t="s">
-        <v>258</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1882,19 +2061,19 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C23" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="D23" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E23" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="F23" t="s">
-        <v>250</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1902,19 +2081,19 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="D24" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E24" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="F24" t="s">
-        <v>259</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1922,19 +2101,19 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E25" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="F25" t="s">
-        <v>260</v>
+        <v>307</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1942,19 +2121,19 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E26" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="F26" t="s">
-        <v>260</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1962,19 +2141,19 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="D27" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E27" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="F27" t="s">
-        <v>261</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1982,19 +2161,19 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E28" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="F28" t="s">
-        <v>262</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -2002,19 +2181,19 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E29" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="F29" t="s">
-        <v>263</v>
+        <v>310</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -2022,19 +2201,19 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E30" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="F30" t="s">
-        <v>264</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -2042,19 +2221,19 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D31" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E31" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="F31" t="s">
-        <v>265</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -2062,19 +2241,19 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D32" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="F32" t="s">
-        <v>266</v>
+        <v>313</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -2082,19 +2261,19 @@
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D33" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E33" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="F33" t="s">
-        <v>267</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -2102,19 +2281,19 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E34" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="F34" t="s">
-        <v>268</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -2122,19 +2301,19 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D35" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E35" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="F35" t="s">
-        <v>269</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -2142,19 +2321,19 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D36" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E36" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="F36" t="s">
-        <v>270</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -2162,19 +2341,19 @@
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D37" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E37" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="F37" t="s">
-        <v>271</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -2182,19 +2361,19 @@
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D38" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E38" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="F38" t="s">
-        <v>272</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -2202,19 +2381,19 @@
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D39" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E39" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="F39" t="s">
-        <v>273</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -2222,19 +2401,19 @@
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E40" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="F40" t="s">
-        <v>274</v>
+        <v>321</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -2242,19 +2421,19 @@
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D41" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E41" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="F41" t="s">
-        <v>275</v>
+        <v>322</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -2262,19 +2441,19 @@
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E42" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="F42" t="s">
-        <v>276</v>
+        <v>323</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -2282,19 +2461,19 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E43" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="F43" t="s">
-        <v>277</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -2302,19 +2481,19 @@
         <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E44" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="F44" t="s">
-        <v>278</v>
+        <v>325</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -2322,19 +2501,19 @@
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C45" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D45" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E45" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="F45" t="s">
-        <v>279</v>
+        <v>326</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -2342,19 +2521,19 @@
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C46" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E46" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="F46" t="s">
-        <v>280</v>
+        <v>327</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -2362,19 +2541,19 @@
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D47" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E47" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="F47" t="s">
-        <v>281</v>
+        <v>328</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -2382,19 +2561,19 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C48" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E48" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="F48" t="s">
-        <v>282</v>
+        <v>329</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -2402,19 +2581,19 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C49" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E49" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="F49" t="s">
-        <v>283</v>
+        <v>330</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -2422,19 +2601,19 @@
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C50" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E50" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="F50" t="s">
-        <v>284</v>
+        <v>331</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -2442,19 +2621,19 @@
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E51" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="F51" t="s">
-        <v>285</v>
+        <v>332</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -2462,19 +2641,19 @@
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E52" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="F52" t="s">
-        <v>286</v>
+        <v>333</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -2482,19 +2661,19 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D53" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E53" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="F53" t="s">
-        <v>287</v>
+        <v>334</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -2502,19 +2681,19 @@
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C54" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D54" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E54" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="F54" t="s">
-        <v>288</v>
+        <v>335</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -2522,19 +2701,19 @@
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D55" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E55" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="F55" t="s">
-        <v>289</v>
+        <v>336</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
@@ -2542,19 +2721,19 @@
         <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D56" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E56" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="F56" t="s">
-        <v>290</v>
+        <v>337</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
@@ -2562,19 +2741,19 @@
         <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C57" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D57" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E57" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="F57" t="s">
-        <v>291</v>
+        <v>338</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -2582,19 +2761,19 @@
         <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C58" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D58" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E58" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="F58" t="s">
-        <v>292</v>
+        <v>339</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
@@ -2602,19 +2781,19 @@
         <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C59" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E59" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="F59" t="s">
-        <v>293</v>
+        <v>340</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -2622,19 +2801,19 @@
         <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C60" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D60" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E60" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="F60" t="s">
-        <v>294</v>
+        <v>341</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -2642,19 +2821,19 @@
         <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C61" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D61" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E61" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="F61" t="s">
-        <v>295</v>
+        <v>342</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -2662,19 +2841,19 @@
         <v>66</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C62" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D62" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E62" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="F62" t="s">
-        <v>296</v>
+        <v>343</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -2682,19 +2861,19 @@
         <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C63" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E63" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="F63" t="s">
-        <v>297</v>
+        <v>344</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -2702,19 +2881,19 @@
         <v>68</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C64" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D64" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E64" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="F64" t="s">
-        <v>298</v>
+        <v>345</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
@@ -2722,19 +2901,19 @@
         <v>69</v>
       </c>
       <c r="B65" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C65" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D65" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E65" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="F65" t="s">
-        <v>299</v>
+        <v>346</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
@@ -2742,19 +2921,19 @@
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C66" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E66" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="F66" t="s">
-        <v>300</v>
+        <v>347</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
@@ -2762,19 +2941,19 @@
         <v>71</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C67" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D67" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E67" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="F67" t="s">
-        <v>301</v>
+        <v>348</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
@@ -2782,19 +2961,19 @@
         <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C68" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D68" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E68" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="F68" t="s">
-        <v>302</v>
+        <v>349</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
@@ -2802,19 +2981,19 @@
         <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C69" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D69" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E69" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="F69" t="s">
-        <v>303</v>
+        <v>350</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.35">
@@ -2822,19 +3001,19 @@
         <v>74</v>
       </c>
       <c r="B70" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C70" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D70" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E70" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="F70" t="s">
-        <v>304</v>
+        <v>351</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.35">
@@ -2842,19 +3021,19 @@
         <v>75</v>
       </c>
       <c r="B71" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D71" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E71" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="F71" t="s">
-        <v>305</v>
+        <v>352</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.35">
@@ -2862,19 +3041,19 @@
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C72" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D72" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E72" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="F72" t="s">
-        <v>306</v>
+        <v>353</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.35">
@@ -2882,19 +3061,19 @@
         <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C73" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D73" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E73" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="F73" t="s">
-        <v>307</v>
+        <v>354</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -2902,19 +3081,19 @@
         <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C74" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D74" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E74" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="F74" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.35">
@@ -2922,19 +3101,19 @@
         <v>79</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C75" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D75" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E75" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="F75" t="s">
-        <v>309</v>
+        <v>356</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.35">
@@ -2942,19 +3121,19 @@
         <v>80</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C76" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D76" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E76" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="F76" t="s">
-        <v>310</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.35">
@@ -2962,19 +3141,19 @@
         <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C77" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D77" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E77" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="F77" t="s">
-        <v>311</v>
+        <v>358</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -2982,19 +3161,19 @@
         <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C78" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D78" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E78" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="F78" t="s">
-        <v>312</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.35">
@@ -3002,19 +3181,19 @@
         <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C79" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D79" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E79" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="F79" t="s">
-        <v>313</v>
+        <v>360</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.35">
@@ -3022,19 +3201,19 @@
         <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C80" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D80" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E80" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="F80" t="s">
-        <v>314</v>
+        <v>361</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
@@ -3042,19 +3221,19 @@
         <v>85</v>
       </c>
       <c r="B81" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C81" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D81" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E81" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="F81" t="s">
-        <v>315</v>
+        <v>362</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
@@ -3062,19 +3241,19 @@
         <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C82" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D82" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E82" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="F82" t="s">
-        <v>316</v>
+        <v>363</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
@@ -3082,19 +3261,19 @@
         <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C83" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D83" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E83" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="F83" t="s">
-        <v>317</v>
+        <v>364</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.35">
@@ -3102,19 +3281,19 @@
         <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C84" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D84" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E84" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="F84" t="s">
-        <v>318</v>
+        <v>365</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
@@ -3122,19 +3301,19 @@
         <v>89</v>
       </c>
       <c r="B85" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C85" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D85" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E85" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="F85" t="s">
-        <v>319</v>
+        <v>366</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
@@ -3142,19 +3321,19 @@
         <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C86" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D86" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E86" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="F86" t="s">
-        <v>320</v>
+        <v>367</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
@@ -3162,19 +3341,19 @@
         <v>91</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C87" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D87" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E87" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="F87" t="s">
-        <v>321</v>
+        <v>368</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
@@ -3182,19 +3361,19 @@
         <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C88" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="D88" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E88" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="F88" t="s">
-        <v>322</v>
+        <v>369</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
@@ -3202,19 +3381,19 @@
         <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C89" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="D89" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E89" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="F89" t="s">
-        <v>323</v>
+        <v>370</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -3222,19 +3401,19 @@
         <v>94</v>
       </c>
       <c r="B90" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C90" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="D90" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E90" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="F90" t="s">
-        <v>324</v>
+        <v>371</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -3242,19 +3421,19 @@
         <v>95</v>
       </c>
       <c r="B91" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C91" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="D91" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E91" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="F91" t="s">
-        <v>325</v>
+        <v>372</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
@@ -3262,19 +3441,19 @@
         <v>96</v>
       </c>
       <c r="B92" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C92" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="D92" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E92" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="F92" t="s">
-        <v>326</v>
+        <v>373</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -3282,19 +3461,19 @@
         <v>97</v>
       </c>
       <c r="B93" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C93" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="D93" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E93" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="F93" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -3302,19 +3481,19 @@
         <v>98</v>
       </c>
       <c r="B94" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C94" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="D94" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E94" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="F94" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -3322,19 +3501,19 @@
         <v>99</v>
       </c>
       <c r="B95" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C95" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D95" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E95" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="F95" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -3342,19 +3521,19 @@
         <v>100</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C96" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="D96" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E96" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="F96" t="s">
-        <v>328</v>
+        <v>375</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
@@ -3362,19 +3541,19 @@
         <v>101</v>
       </c>
       <c r="B97" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="C97" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="D97" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E97" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="F97" t="s">
-        <v>329</v>
+        <v>376</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
@@ -3382,19 +3561,19 @@
         <v>102</v>
       </c>
       <c r="B98" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="C98" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="D98" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E98" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="F98" t="s">
-        <v>330</v>
+        <v>377</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -3402,19 +3581,19 @@
         <v>103</v>
       </c>
       <c r="B99" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="C99" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="D99" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E99" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="F99" t="s">
-        <v>331</v>
+        <v>378</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
@@ -3422,19 +3601,19 @@
         <v>104</v>
       </c>
       <c r="B100" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="C100" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="D100" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E100" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="F100" t="s">
-        <v>332</v>
+        <v>379</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
@@ -3442,19 +3621,19 @@
         <v>105</v>
       </c>
       <c r="B101" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="C101" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="D101" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E101" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="F101" t="s">
-        <v>333</v>
+        <v>380</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
@@ -3462,19 +3641,19 @@
         <v>106</v>
       </c>
       <c r="B102" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="C102" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
       <c r="D102" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E102" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="F102" t="s">
-        <v>334</v>
+        <v>381</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
@@ -3482,19 +3661,479 @@
         <v>107</v>
       </c>
       <c r="B103" t="s">
+        <v>131</v>
+      </c>
+      <c r="C103" t="s">
+        <v>154</v>
+      </c>
+      <c r="D103" t="s">
+        <v>168</v>
+      </c>
+      <c r="E103" t="s">
+        <v>267</v>
+      </c>
+      <c r="F103" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>108</v>
       </c>
-      <c r="C103" t="s">
-        <v>131</v>
-      </c>
-      <c r="D103" t="s">
-        <v>144</v>
-      </c>
-      <c r="E103" t="s">
-        <v>243</v>
-      </c>
-      <c r="F103" t="s">
-        <v>335</v>
+      <c r="B104" t="s">
+        <v>133</v>
+      </c>
+      <c r="C104" t="s">
+        <v>166</v>
+      </c>
+      <c r="D104" t="s">
+        <v>168</v>
+      </c>
+      <c r="E104" t="s">
+        <v>268</v>
+      </c>
+      <c r="F104" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>109</v>
+      </c>
+      <c r="B105" t="s">
+        <v>133</v>
+      </c>
+      <c r="C105" t="s">
+        <v>166</v>
+      </c>
+      <c r="D105" t="s">
+        <v>168</v>
+      </c>
+      <c r="E105" t="s">
+        <v>269</v>
+      </c>
+      <c r="F105" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>110</v>
+      </c>
+      <c r="B106" t="s">
+        <v>133</v>
+      </c>
+      <c r="C106" t="s">
+        <v>166</v>
+      </c>
+      <c r="D106" t="s">
+        <v>168</v>
+      </c>
+      <c r="E106" t="s">
+        <v>270</v>
+      </c>
+      <c r="F106" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>111</v>
+      </c>
+      <c r="B107" t="s">
+        <v>133</v>
+      </c>
+      <c r="C107" t="s">
+        <v>166</v>
+      </c>
+      <c r="D107" t="s">
+        <v>168</v>
+      </c>
+      <c r="E107" t="s">
+        <v>271</v>
+      </c>
+      <c r="F107" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>112</v>
+      </c>
+      <c r="B108" t="s">
+        <v>133</v>
+      </c>
+      <c r="C108" t="s">
+        <v>166</v>
+      </c>
+      <c r="D108" t="s">
+        <v>168</v>
+      </c>
+      <c r="E108" t="s">
+        <v>272</v>
+      </c>
+      <c r="F108" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>113</v>
+      </c>
+      <c r="B109" t="s">
+        <v>133</v>
+      </c>
+      <c r="C109" t="s">
+        <v>166</v>
+      </c>
+      <c r="D109" t="s">
+        <v>168</v>
+      </c>
+      <c r="E109" t="s">
+        <v>273</v>
+      </c>
+      <c r="F109" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>114</v>
+      </c>
+      <c r="B110" t="s">
+        <v>133</v>
+      </c>
+      <c r="C110" t="s">
+        <v>166</v>
+      </c>
+      <c r="D110" t="s">
+        <v>168</v>
+      </c>
+      <c r="E110" t="s">
+        <v>274</v>
+      </c>
+      <c r="F110" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>115</v>
+      </c>
+      <c r="B111" t="s">
+        <v>133</v>
+      </c>
+      <c r="C111" t="s">
+        <v>166</v>
+      </c>
+      <c r="D111" t="s">
+        <v>168</v>
+      </c>
+      <c r="E111" t="s">
+        <v>275</v>
+      </c>
+      <c r="F111" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>116</v>
+      </c>
+      <c r="B112" t="s">
+        <v>133</v>
+      </c>
+      <c r="C112" t="s">
+        <v>166</v>
+      </c>
+      <c r="D112" t="s">
+        <v>168</v>
+      </c>
+      <c r="E112" t="s">
+        <v>276</v>
+      </c>
+      <c r="F112" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>117</v>
+      </c>
+      <c r="B113" t="s">
+        <v>133</v>
+      </c>
+      <c r="C113" t="s">
+        <v>166</v>
+      </c>
+      <c r="D113" t="s">
+        <v>168</v>
+      </c>
+      <c r="E113" t="s">
+        <v>277</v>
+      </c>
+      <c r="F113" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>118</v>
+      </c>
+      <c r="B114" t="s">
+        <v>133</v>
+      </c>
+      <c r="C114" t="s">
+        <v>166</v>
+      </c>
+      <c r="D114" t="s">
+        <v>168</v>
+      </c>
+      <c r="E114" t="s">
+        <v>278</v>
+      </c>
+      <c r="F114" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>119</v>
+      </c>
+      <c r="B115" t="s">
+        <v>133</v>
+      </c>
+      <c r="C115" t="s">
+        <v>166</v>
+      </c>
+      <c r="D115" t="s">
+        <v>168</v>
+      </c>
+      <c r="E115" t="s">
+        <v>279</v>
+      </c>
+      <c r="F115" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>120</v>
+      </c>
+      <c r="B116" t="s">
+        <v>133</v>
+      </c>
+      <c r="C116" t="s">
+        <v>166</v>
+      </c>
+      <c r="D116" t="s">
+        <v>168</v>
+      </c>
+      <c r="E116" t="s">
+        <v>280</v>
+      </c>
+      <c r="F116" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>121</v>
+      </c>
+      <c r="B117" t="s">
+        <v>133</v>
+      </c>
+      <c r="C117" t="s">
+        <v>166</v>
+      </c>
+      <c r="D117" t="s">
+        <v>168</v>
+      </c>
+      <c r="E117" t="s">
+        <v>281</v>
+      </c>
+      <c r="F117" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>122</v>
+      </c>
+      <c r="B118" t="s">
+        <v>133</v>
+      </c>
+      <c r="C118" t="s">
+        <v>166</v>
+      </c>
+      <c r="D118" t="s">
+        <v>168</v>
+      </c>
+      <c r="E118" t="s">
+        <v>282</v>
+      </c>
+      <c r="F118" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>123</v>
+      </c>
+      <c r="B119" t="s">
+        <v>133</v>
+      </c>
+      <c r="C119" t="s">
+        <v>166</v>
+      </c>
+      <c r="D119" t="s">
+        <v>168</v>
+      </c>
+      <c r="E119" t="s">
+        <v>283</v>
+      </c>
+      <c r="F119" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>124</v>
+      </c>
+      <c r="B120" t="s">
+        <v>133</v>
+      </c>
+      <c r="C120" t="s">
+        <v>166</v>
+      </c>
+      <c r="D120" t="s">
+        <v>168</v>
+      </c>
+      <c r="E120" t="s">
+        <v>284</v>
+      </c>
+      <c r="F120" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>125</v>
+      </c>
+      <c r="B121" t="s">
+        <v>133</v>
+      </c>
+      <c r="C121" t="s">
+        <v>166</v>
+      </c>
+      <c r="D121" t="s">
+        <v>168</v>
+      </c>
+      <c r="E121" t="s">
+        <v>285</v>
+      </c>
+      <c r="F121" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>126</v>
+      </c>
+      <c r="B122" t="s">
+        <v>133</v>
+      </c>
+      <c r="C122" t="s">
+        <v>166</v>
+      </c>
+      <c r="D122" t="s">
+        <v>168</v>
+      </c>
+      <c r="E122" t="s">
+        <v>286</v>
+      </c>
+      <c r="F122" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>127</v>
+      </c>
+      <c r="B123" t="s">
+        <v>133</v>
+      </c>
+      <c r="C123" t="s">
+        <v>166</v>
+      </c>
+      <c r="D123" t="s">
+        <v>168</v>
+      </c>
+      <c r="E123" t="s">
+        <v>287</v>
+      </c>
+      <c r="F123" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>128</v>
+      </c>
+      <c r="B124" t="s">
+        <v>133</v>
+      </c>
+      <c r="C124" t="s">
+        <v>166</v>
+      </c>
+      <c r="D124" t="s">
+        <v>168</v>
+      </c>
+      <c r="E124" t="s">
+        <v>288</v>
+      </c>
+      <c r="F124" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>129</v>
+      </c>
+      <c r="B125" t="s">
+        <v>133</v>
+      </c>
+      <c r="C125" t="s">
+        <v>166</v>
+      </c>
+      <c r="D125" t="s">
+        <v>168</v>
+      </c>
+      <c r="E125" t="s">
+        <v>289</v>
+      </c>
+      <c r="F125" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>130</v>
+      </c>
+      <c r="B126" t="s">
+        <v>133</v>
+      </c>
+      <c r="C126" t="s">
+        <v>166</v>
+      </c>
+      <c r="D126" t="s">
+        <v>168</v>
+      </c>
+      <c r="E126" t="s">
+        <v>290</v>
+      </c>
+      <c r="F126" t="s">
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>